<commit_message>
Overall enhancement for test data supplying
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/VehicleInsuranceCalcualator_TestData.xlsx
+++ b/src/test/resources/testData/VehicleInsuranceCalcualator_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\eclipse-workspace\Training.InsuranceCalculator\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19163\seleniumArchitecture\InsuranceCalc\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0788422-D740-4539-B247-27CABBD8CD2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E516A8E4-E898-4D52-8BB3-8D6D0F379273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A380FA76-9CC6-4F4D-9280-5EC28A377BCB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A380FA76-9CC6-4F4D-9280-5EC28A377BCB}"/>
   </bookViews>
   <sheets>
     <sheet name="InsurancePremium" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>TC No</t>
   </si>
@@ -263,9 +263,6 @@
   </si>
   <si>
     <t>12/12/1956</t>
-  </si>
-  <si>
-    <t>12/12/2020</t>
   </si>
   <si>
     <t>12/12/2025</t>
@@ -683,35 +680,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255CEB0C-D017-479D-8DDE-08C67B4AF72D}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="18" width="19.77734375" customWidth="1"/>
-    <col min="19" max="19" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="19.77734375" customWidth="1"/>
-    <col min="22" max="22" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.44140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="19.7109375" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="19.7109375" customWidth="1"/>
+    <col min="22" max="22" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -797,7 +794,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -883,7 +880,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -942,7 +939,7 @@
         <v>32</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U3" t="s">
         <v>66</v>
@@ -969,7 +966,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1028,7 +1025,7 @@
         <v>32</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U4" t="s">
         <v>67</v>
@@ -1069,9 +1066,9 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1079,7 +1076,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1087,7 +1084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>

</xml_diff>